<commit_message>
Automático: Datos procesados actualizados
</commit_message>
<xml_diff>
--- a/output/datos_transformados.xlsx
+++ b/output/datos_transformados.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,20 +445,25 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>producto</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Nombre proveedor</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Zona</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Reclamo</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Venta</t>
         </is>
@@ -470,18 +475,23 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>COOPERATIVA HORTOFRUTICOLA CARTAYA</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Z1</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
       <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -491,18 +501,23 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>COOPERATIVA HORTOFRUTICOLA CARTAYA</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Z2</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>648</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>28519.8</v>
       </c>
     </row>
@@ -512,18 +527,23 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>COOPERATIVA HORTOFRUTICOLA CARTAYA</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Z3</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
       <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
         <v>21060</v>
       </c>
     </row>
@@ -533,18 +553,23 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>COOPERATIVA HORTOFRUTICOLA CARTAYA</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Z4</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>636</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>32955</v>
       </c>
     </row>
@@ -554,18 +579,23 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>FRESLUCENA, S.A.</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>Z1</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
       <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -575,18 +605,23 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>FRESLUCENA, S.A.</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Z2</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
       <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -596,18 +631,23 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>FRESLUCENA, S.A.</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Z3</t>
         </is>
       </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
       <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -617,18 +657,23 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>FRESLUCENA, S.A.</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Z4</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
       <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -638,18 +683,23 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>ONUBAFRUIT</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Z1</t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
       <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -659,18 +709,23 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>ONUBAFRUIT</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>Z2</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>648</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>38479.8</v>
       </c>
     </row>
@@ -680,18 +735,23 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>ONUBAFRUIT</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>Z3</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
       <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
         <v>22509</v>
       </c>
     </row>
@@ -701,18 +761,23 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>ONUBAFRUIT</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>Z4</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>891</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>43590</v>
       </c>
     </row>
@@ -722,18 +787,23 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>S.A.T CONDADO DE HUELVA</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>Z1</t>
         </is>
       </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
       <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -743,18 +813,23 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>S.A.T CONDADO DE HUELVA</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>Z2</t>
         </is>
       </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
       <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
         <v>283.5</v>
       </c>
     </row>
@@ -764,18 +839,23 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>S.A.T CONDADO DE HUELVA</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>Z3</t>
         </is>
       </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
       <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -785,18 +865,23 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>S.A.T CONDADO DE HUELVA</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>Z4</t>
         </is>
       </c>
-      <c r="D17" t="n">
-        <v>0</v>
-      </c>
       <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -806,18 +891,23 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>S.C.A. COSTA DE HUELVA</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>Z1</t>
         </is>
       </c>
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
       <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -827,18 +917,23 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
           <t>S.C.A. COSTA DE HUELVA</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>Z2</t>
         </is>
       </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
       <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
         <v>3043.5</v>
       </c>
     </row>
@@ -848,18 +943,23 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
           <t>S.C.A. COSTA DE HUELVA</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>Z3</t>
         </is>
       </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
       <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
         <v>1449</v>
       </c>
     </row>
@@ -869,18 +969,23 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>S.C.A. COSTA DE HUELVA</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>Z4</t>
         </is>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>255</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>4560</v>
       </c>
     </row>
@@ -890,18 +995,23 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>S.C.A. NUESTRA SRA. LA BELLA</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>Z1</t>
         </is>
       </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
       <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -911,18 +1021,23 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
           <t>S.C.A. NUESTRA SRA. LA BELLA</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>Z2</t>
         </is>
       </c>
-      <c r="D23" t="n">
-        <v>0</v>
-      </c>
       <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
         <v>6633</v>
       </c>
     </row>
@@ -932,18 +1047,23 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>S.C.A. NUESTRA SRA. LA BELLA</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>Z3</t>
         </is>
       </c>
-      <c r="D24" t="n">
-        <v>0</v>
-      </c>
       <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -953,18 +1073,23 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
           <t>S.C.A. NUESTRA SRA. LA BELLA</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>Z4</t>
         </is>
       </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
       <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
         <v>6075</v>
       </c>
     </row>
@@ -974,18 +1099,23 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
           <t>VARIOS</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>Z1</t>
         </is>
       </c>
-      <c r="D26" t="n">
-        <v>0</v>
-      </c>
       <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -995,18 +1125,23 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
           <t>VARIOS</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>Z2</t>
         </is>
       </c>
-      <c r="D27" t="n">
-        <v>0</v>
-      </c>
       <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1016,18 +1151,23 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
           <t>VARIOS</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>Z3</t>
         </is>
       </c>
-      <c r="D28" t="n">
-        <v>0</v>
-      </c>
       <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1037,18 +1177,23 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>DESCONOCIDO</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
           <t>VARIOS</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>Z4</t>
         </is>
       </c>
-      <c r="D29" t="n">
-        <v>0</v>
-      </c>
       <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>